<commit_message>
Updated to work on latest Dynamics version
</commit_message>
<xml_diff>
--- a/TC_CreatePriceList/Main.rvl.xlsx
+++ b/TC_CreatePriceList/Main.rvl.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="167">
   <si>
     <t>Flow</t>
   </si>
@@ -507,6 +507,15 @@
   </si>
   <si>
     <t>PriceListItems</t>
+  </si>
+  <si>
+    <t>Pricing_information</t>
+  </si>
+  <si>
+    <t>Cleanup</t>
+  </si>
+  <si>
+    <t>KillBrowser</t>
   </si>
 </sst>
 </file>
@@ -527,7 +536,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1268">
+  <borders count="1269">
     <border>
       <left/>
       <right/>
@@ -1802,11 +1811,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1268">
+  <cellXfs count="1269">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -3075,6 +3085,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1265" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1266" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1267" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1268" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3787,9 +3798,45 @@
     </row>
     <row r="45">
       <c r="A45" s="238"/>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="239"/>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="240"/>
@@ -3806,7 +3853,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H70"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.453125" customWidth="true"/>
@@ -4238,14 +4285,14 @@
       <c r="A25" s="633"/>
     </row>
     <row r="26">
-      <c r="A26" s="630" t="s">
+      <c r="A26" s="1268" t="s">
         <v>7</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>164</v>
       </c>
       <c r="D26" t="s">
         <v>22</v>
@@ -4261,7 +4308,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="631" t="s">
+      <c r="A27" s="630" t="s">
         <v>7</v>
       </c>
       <c r="B27" t="s">
@@ -4271,463 +4318,486 @@
         <v>117</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="G27" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="632" t="s">
+      <c r="A28" s="631" t="s">
         <v>7</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="C28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" t="s">
+        <v>75</v>
+      </c>
+      <c r="G28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="632" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
         <v>119</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>22</v>
       </c>
-      <c r="E28" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="655" t="s">
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="655" t="s">
         <v>72</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>125</v>
       </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="303"/>
-      <c r="B30" s="304"/>
-      <c r="C30" s="305"/>
-      <c r="D30" s="306"/>
-      <c r="E30" s="307"/>
-      <c r="F30" s="308"/>
-      <c r="G30" s="309"/>
-      <c r="H30" s="310"/>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="311"/>
-      <c r="B31" s="312"/>
-      <c r="C31" s="313"/>
-      <c r="D31" s="314"/>
-      <c r="E31" s="315"/>
-      <c r="F31" s="316"/>
-      <c r="G31" s="317"/>
-      <c r="H31" s="318"/>
+      <c r="A31" s="303"/>
+      <c r="B31" s="304"/>
+      <c r="C31" s="305"/>
+      <c r="D31" s="306"/>
+      <c r="E31" s="307"/>
+      <c r="F31" s="308"/>
+      <c r="G31" s="309"/>
+      <c r="H31" s="310"/>
     </row>
     <row r="32">
-      <c r="A32" s="319"/>
-      <c r="B32" s="320"/>
-      <c r="C32" s="321"/>
-      <c r="D32" s="322"/>
-      <c r="E32" s="323"/>
-      <c r="F32" s="324"/>
-      <c r="G32" s="325"/>
-      <c r="H32" s="326"/>
+      <c r="A32" s="311"/>
+      <c r="B32" s="312"/>
+      <c r="C32" s="313"/>
+      <c r="D32" s="314"/>
+      <c r="E32" s="315"/>
+      <c r="F32" s="316"/>
+      <c r="G32" s="317"/>
+      <c r="H32" s="318"/>
     </row>
     <row r="33">
-      <c r="A33" s="327"/>
-      <c r="B33" s="328"/>
-      <c r="C33" s="329"/>
-      <c r="D33" s="330"/>
-      <c r="E33" s="331"/>
-      <c r="F33" s="332"/>
-      <c r="G33" s="333"/>
-      <c r="H33" s="334"/>
+      <c r="A33" s="319"/>
+      <c r="B33" s="320"/>
+      <c r="C33" s="321"/>
+      <c r="D33" s="322"/>
+      <c r="E33" s="323"/>
+      <c r="F33" s="324"/>
+      <c r="G33" s="325"/>
+      <c r="H33" s="326"/>
     </row>
     <row r="34">
-      <c r="A34" s="335"/>
-      <c r="B34" s="336"/>
-      <c r="C34" s="337"/>
-      <c r="D34" s="338"/>
-      <c r="E34" s="339"/>
-      <c r="F34" s="340"/>
-      <c r="G34" s="341"/>
-      <c r="H34" s="342"/>
+      <c r="A34" s="327"/>
+      <c r="B34" s="328"/>
+      <c r="C34" s="329"/>
+      <c r="D34" s="330"/>
+      <c r="E34" s="331"/>
+      <c r="F34" s="332"/>
+      <c r="G34" s="333"/>
+      <c r="H34" s="334"/>
     </row>
     <row r="35">
-      <c r="A35" s="343"/>
-      <c r="B35" s="344"/>
-      <c r="C35" s="345"/>
-      <c r="D35" s="346"/>
-      <c r="E35" s="347"/>
-      <c r="F35" s="348"/>
-      <c r="G35" s="349"/>
-      <c r="H35" s="350"/>
+      <c r="A35" s="335"/>
+      <c r="B35" s="336"/>
+      <c r="C35" s="337"/>
+      <c r="D35" s="338"/>
+      <c r="E35" s="339"/>
+      <c r="F35" s="340"/>
+      <c r="G35" s="341"/>
+      <c r="H35" s="342"/>
     </row>
     <row r="36">
-      <c r="A36" s="351"/>
-      <c r="B36" s="352"/>
-      <c r="C36" s="353"/>
-      <c r="D36" s="354"/>
-      <c r="E36" s="355"/>
-      <c r="F36" s="356"/>
-      <c r="G36" s="357"/>
-      <c r="H36" s="358"/>
+      <c r="A36" s="343"/>
+      <c r="B36" s="344"/>
+      <c r="C36" s="345"/>
+      <c r="D36" s="346"/>
+      <c r="E36" s="347"/>
+      <c r="F36" s="348"/>
+      <c r="G36" s="349"/>
+      <c r="H36" s="350"/>
     </row>
     <row r="37">
-      <c r="A37" s="359"/>
-      <c r="B37" s="360"/>
-      <c r="C37" s="361"/>
-      <c r="D37" s="362"/>
-      <c r="E37" s="363"/>
-      <c r="F37" s="364"/>
-      <c r="G37" s="365"/>
-      <c r="H37" s="366"/>
+      <c r="A37" s="351"/>
+      <c r="B37" s="352"/>
+      <c r="C37" s="353"/>
+      <c r="D37" s="354"/>
+      <c r="E37" s="355"/>
+      <c r="F37" s="356"/>
+      <c r="G37" s="357"/>
+      <c r="H37" s="358"/>
     </row>
     <row r="38">
-      <c r="A38" s="367"/>
-      <c r="B38" s="368"/>
-      <c r="C38" s="369"/>
-      <c r="D38" s="370"/>
-      <c r="E38" s="371"/>
-      <c r="F38" s="372"/>
-      <c r="G38" s="373"/>
-      <c r="H38" s="374"/>
+      <c r="A38" s="359"/>
+      <c r="B38" s="360"/>
+      <c r="C38" s="361"/>
+      <c r="D38" s="362"/>
+      <c r="E38" s="363"/>
+      <c r="F38" s="364"/>
+      <c r="G38" s="365"/>
+      <c r="H38" s="366"/>
     </row>
     <row r="39">
-      <c r="A39" s="375"/>
-      <c r="B39" s="376"/>
-      <c r="C39" s="377"/>
-      <c r="D39" s="378"/>
-      <c r="E39" s="379"/>
-      <c r="F39" s="380"/>
-      <c r="G39" s="381"/>
-      <c r="H39" s="382"/>
+      <c r="A39" s="367"/>
+      <c r="B39" s="368"/>
+      <c r="C39" s="369"/>
+      <c r="D39" s="370"/>
+      <c r="E39" s="371"/>
+      <c r="F39" s="372"/>
+      <c r="G39" s="373"/>
+      <c r="H39" s="374"/>
     </row>
     <row r="40">
-      <c r="A40" s="383"/>
-      <c r="B40" s="384"/>
-      <c r="C40" s="385"/>
-      <c r="D40" s="386"/>
-      <c r="E40" s="387"/>
-      <c r="F40" s="388"/>
-      <c r="G40" s="389"/>
-      <c r="H40" s="390"/>
+      <c r="A40" s="375"/>
+      <c r="B40" s="376"/>
+      <c r="C40" s="377"/>
+      <c r="D40" s="378"/>
+      <c r="E40" s="379"/>
+      <c r="F40" s="380"/>
+      <c r="G40" s="381"/>
+      <c r="H40" s="382"/>
     </row>
     <row r="41">
-      <c r="A41" s="391"/>
-      <c r="B41" s="392"/>
-      <c r="C41" s="393"/>
-      <c r="D41" s="394"/>
-      <c r="E41" s="395"/>
-      <c r="F41" s="396"/>
-      <c r="G41" s="397"/>
-      <c r="H41" s="398"/>
+      <c r="A41" s="383"/>
+      <c r="B41" s="384"/>
+      <c r="C41" s="385"/>
+      <c r="D41" s="386"/>
+      <c r="E41" s="387"/>
+      <c r="F41" s="388"/>
+      <c r="G41" s="389"/>
+      <c r="H41" s="390"/>
     </row>
     <row r="42">
-      <c r="A42" s="399"/>
-      <c r="B42" s="400"/>
-      <c r="C42" s="401"/>
-      <c r="D42" s="402"/>
-      <c r="E42" s="403"/>
-      <c r="F42" s="404"/>
-      <c r="G42" s="405"/>
-      <c r="H42" s="406"/>
+      <c r="A42" s="391"/>
+      <c r="B42" s="392"/>
+      <c r="C42" s="393"/>
+      <c r="D42" s="394"/>
+      <c r="E42" s="395"/>
+      <c r="F42" s="396"/>
+      <c r="G42" s="397"/>
+      <c r="H42" s="398"/>
     </row>
     <row r="43">
-      <c r="A43" s="407"/>
-      <c r="B43" s="408"/>
-      <c r="C43" s="409"/>
-      <c r="D43" s="410"/>
-      <c r="E43" s="411"/>
-      <c r="F43" s="412"/>
-      <c r="G43" s="413"/>
-      <c r="H43" s="414"/>
+      <c r="A43" s="399"/>
+      <c r="B43" s="400"/>
+      <c r="C43" s="401"/>
+      <c r="D43" s="402"/>
+      <c r="E43" s="403"/>
+      <c r="F43" s="404"/>
+      <c r="G43" s="405"/>
+      <c r="H43" s="406"/>
     </row>
     <row r="44">
-      <c r="A44" s="415"/>
-      <c r="B44" s="416"/>
-      <c r="C44" s="417"/>
-      <c r="D44" s="418"/>
-      <c r="E44" s="419"/>
-      <c r="F44" s="420"/>
-      <c r="G44" s="421"/>
-      <c r="H44" s="422"/>
+      <c r="A44" s="407"/>
+      <c r="B44" s="408"/>
+      <c r="C44" s="409"/>
+      <c r="D44" s="410"/>
+      <c r="E44" s="411"/>
+      <c r="F44" s="412"/>
+      <c r="G44" s="413"/>
+      <c r="H44" s="414"/>
     </row>
     <row r="45">
-      <c r="A45" s="423"/>
-      <c r="B45" s="424"/>
-      <c r="C45" s="425"/>
-      <c r="D45" s="426"/>
-      <c r="E45" s="427"/>
-      <c r="F45" s="428"/>
-      <c r="G45" s="429"/>
-      <c r="H45" s="430"/>
+      <c r="A45" s="415"/>
+      <c r="B45" s="416"/>
+      <c r="C45" s="417"/>
+      <c r="D45" s="418"/>
+      <c r="E45" s="419"/>
+      <c r="F45" s="420"/>
+      <c r="G45" s="421"/>
+      <c r="H45" s="422"/>
     </row>
     <row r="46">
-      <c r="A46" s="431"/>
-      <c r="B46" s="432"/>
-      <c r="C46" s="433"/>
-      <c r="D46" s="434"/>
-      <c r="E46" s="435"/>
-      <c r="F46" s="436"/>
-      <c r="G46" s="437"/>
-      <c r="H46" s="438"/>
+      <c r="A46" s="423"/>
+      <c r="B46" s="424"/>
+      <c r="C46" s="425"/>
+      <c r="D46" s="426"/>
+      <c r="E46" s="427"/>
+      <c r="F46" s="428"/>
+      <c r="G46" s="429"/>
+      <c r="H46" s="430"/>
     </row>
     <row r="47">
-      <c r="A47" s="439"/>
-      <c r="B47" s="440"/>
-      <c r="C47" s="441"/>
-      <c r="D47" s="442"/>
-      <c r="E47" s="443"/>
-      <c r="F47" s="444"/>
-      <c r="G47" s="445"/>
-      <c r="H47" s="446"/>
+      <c r="A47" s="431"/>
+      <c r="B47" s="432"/>
+      <c r="C47" s="433"/>
+      <c r="D47" s="434"/>
+      <c r="E47" s="435"/>
+      <c r="F47" s="436"/>
+      <c r="G47" s="437"/>
+      <c r="H47" s="438"/>
     </row>
     <row r="48">
-      <c r="A48" s="447"/>
-      <c r="B48" s="448"/>
-      <c r="C48" s="449"/>
-      <c r="D48" s="450"/>
-      <c r="E48" s="451"/>
-      <c r="F48" s="452"/>
-      <c r="G48" s="453"/>
-      <c r="H48" s="454"/>
+      <c r="A48" s="439"/>
+      <c r="B48" s="440"/>
+      <c r="C48" s="441"/>
+      <c r="D48" s="442"/>
+      <c r="E48" s="443"/>
+      <c r="F48" s="444"/>
+      <c r="G48" s="445"/>
+      <c r="H48" s="446"/>
     </row>
     <row r="49">
-      <c r="A49" s="455"/>
-      <c r="B49" s="456"/>
-      <c r="C49" s="457"/>
-      <c r="D49" s="458"/>
-      <c r="E49" s="459"/>
-      <c r="F49" s="460"/>
-      <c r="G49" s="461"/>
-      <c r="H49" s="462"/>
+      <c r="A49" s="447"/>
+      <c r="B49" s="448"/>
+      <c r="C49" s="449"/>
+      <c r="D49" s="450"/>
+      <c r="E49" s="451"/>
+      <c r="F49" s="452"/>
+      <c r="G49" s="453"/>
+      <c r="H49" s="454"/>
     </row>
     <row r="50">
-      <c r="A50" s="463"/>
-      <c r="B50" s="464"/>
-      <c r="C50" s="465"/>
-      <c r="D50" s="466"/>
-      <c r="E50" s="467"/>
-      <c r="F50" s="468"/>
-      <c r="G50" s="469"/>
-      <c r="H50" s="470"/>
+      <c r="A50" s="455"/>
+      <c r="B50" s="456"/>
+      <c r="C50" s="457"/>
+      <c r="D50" s="458"/>
+      <c r="E50" s="459"/>
+      <c r="F50" s="460"/>
+      <c r="G50" s="461"/>
+      <c r="H50" s="462"/>
     </row>
     <row r="51">
-      <c r="A51" s="471"/>
-      <c r="B51" s="472"/>
-      <c r="C51" s="473"/>
-      <c r="D51" s="474"/>
-      <c r="E51" s="475"/>
-      <c r="F51" s="476"/>
-      <c r="G51" s="477"/>
-      <c r="H51" s="478"/>
+      <c r="A51" s="463"/>
+      <c r="B51" s="464"/>
+      <c r="C51" s="465"/>
+      <c r="D51" s="466"/>
+      <c r="E51" s="467"/>
+      <c r="F51" s="468"/>
+      <c r="G51" s="469"/>
+      <c r="H51" s="470"/>
     </row>
     <row r="52">
-      <c r="A52" s="479"/>
-      <c r="B52" s="480"/>
-      <c r="C52" s="481"/>
-      <c r="D52" s="482"/>
-      <c r="E52" s="483"/>
-      <c r="F52" s="484"/>
-      <c r="G52" s="485"/>
-      <c r="H52" s="486"/>
+      <c r="A52" s="471"/>
+      <c r="B52" s="472"/>
+      <c r="C52" s="473"/>
+      <c r="D52" s="474"/>
+      <c r="E52" s="475"/>
+      <c r="F52" s="476"/>
+      <c r="G52" s="477"/>
+      <c r="H52" s="478"/>
     </row>
     <row r="53">
-      <c r="A53" s="487"/>
-      <c r="B53" s="488"/>
-      <c r="C53" s="489"/>
-      <c r="D53" s="490"/>
-      <c r="E53" s="491"/>
-      <c r="F53" s="492"/>
-      <c r="G53" s="493"/>
-      <c r="H53" s="494"/>
+      <c r="A53" s="479"/>
+      <c r="B53" s="480"/>
+      <c r="C53" s="481"/>
+      <c r="D53" s="482"/>
+      <c r="E53" s="483"/>
+      <c r="F53" s="484"/>
+      <c r="G53" s="485"/>
+      <c r="H53" s="486"/>
     </row>
     <row r="54">
-      <c r="A54" s="495"/>
-      <c r="B54" s="496"/>
-      <c r="C54" s="497"/>
-      <c r="D54" s="498"/>
-      <c r="E54" s="499"/>
-      <c r="F54" s="500"/>
-      <c r="G54" s="501"/>
-      <c r="H54" s="502"/>
+      <c r="A54" s="487"/>
+      <c r="B54" s="488"/>
+      <c r="C54" s="489"/>
+      <c r="D54" s="490"/>
+      <c r="E54" s="491"/>
+      <c r="F54" s="492"/>
+      <c r="G54" s="493"/>
+      <c r="H54" s="494"/>
     </row>
     <row r="55">
-      <c r="A55" s="503"/>
-      <c r="B55" s="504"/>
-      <c r="C55" s="505"/>
-      <c r="D55" s="506"/>
-      <c r="E55" s="507"/>
-      <c r="F55" s="508"/>
-      <c r="G55" s="509"/>
-      <c r="H55" s="510"/>
+      <c r="A55" s="495"/>
+      <c r="B55" s="496"/>
+      <c r="C55" s="497"/>
+      <c r="D55" s="498"/>
+      <c r="E55" s="499"/>
+      <c r="F55" s="500"/>
+      <c r="G55" s="501"/>
+      <c r="H55" s="502"/>
     </row>
     <row r="56">
-      <c r="A56" s="511"/>
-      <c r="B56" s="512"/>
-      <c r="C56" s="513"/>
-      <c r="D56" s="514"/>
-      <c r="E56" s="515"/>
-      <c r="F56" s="516"/>
-      <c r="G56" s="517"/>
-      <c r="H56" s="518"/>
+      <c r="A56" s="503"/>
+      <c r="B56" s="504"/>
+      <c r="C56" s="505"/>
+      <c r="D56" s="506"/>
+      <c r="E56" s="507"/>
+      <c r="F56" s="508"/>
+      <c r="G56" s="509"/>
+      <c r="H56" s="510"/>
     </row>
     <row r="57">
-      <c r="A57" s="519"/>
-      <c r="B57" s="520"/>
-      <c r="C57" s="521"/>
-      <c r="D57" s="522"/>
-      <c r="E57" s="523"/>
-      <c r="F57" s="524"/>
-      <c r="G57" s="525"/>
-      <c r="H57" s="526"/>
+      <c r="A57" s="511"/>
+      <c r="B57" s="512"/>
+      <c r="C57" s="513"/>
+      <c r="D57" s="514"/>
+      <c r="E57" s="515"/>
+      <c r="F57" s="516"/>
+      <c r="G57" s="517"/>
+      <c r="H57" s="518"/>
     </row>
     <row r="58">
-      <c r="A58" s="527"/>
-      <c r="B58" s="528"/>
-      <c r="C58" s="529"/>
-      <c r="D58" s="530"/>
-      <c r="E58" s="531"/>
-      <c r="F58" s="532"/>
-      <c r="G58" s="533"/>
-      <c r="H58" s="534"/>
+      <c r="A58" s="519"/>
+      <c r="B58" s="520"/>
+      <c r="C58" s="521"/>
+      <c r="D58" s="522"/>
+      <c r="E58" s="523"/>
+      <c r="F58" s="524"/>
+      <c r="G58" s="525"/>
+      <c r="H58" s="526"/>
     </row>
     <row r="59">
-      <c r="A59" s="535"/>
-      <c r="B59" s="536"/>
-      <c r="C59" s="537"/>
-      <c r="D59" s="538"/>
-      <c r="E59" s="539"/>
-      <c r="F59" s="540"/>
-      <c r="G59" s="541"/>
-      <c r="H59" s="542"/>
+      <c r="A59" s="527"/>
+      <c r="B59" s="528"/>
+      <c r="C59" s="529"/>
+      <c r="D59" s="530"/>
+      <c r="E59" s="531"/>
+      <c r="F59" s="532"/>
+      <c r="G59" s="533"/>
+      <c r="H59" s="534"/>
     </row>
     <row r="60">
-      <c r="A60" s="543"/>
-      <c r="B60" s="544"/>
-      <c r="C60" s="545"/>
-      <c r="D60" s="546"/>
-      <c r="E60" s="547"/>
-      <c r="F60" s="548"/>
-      <c r="G60" s="549"/>
-      <c r="H60" s="550"/>
+      <c r="A60" s="535"/>
+      <c r="B60" s="536"/>
+      <c r="C60" s="537"/>
+      <c r="D60" s="538"/>
+      <c r="E60" s="539"/>
+      <c r="F60" s="540"/>
+      <c r="G60" s="541"/>
+      <c r="H60" s="542"/>
     </row>
     <row r="61">
-      <c r="A61" s="551"/>
-      <c r="B61" s="552"/>
-      <c r="C61" s="553"/>
-      <c r="D61" s="554"/>
-      <c r="E61" s="555"/>
-      <c r="F61" s="556"/>
-      <c r="G61" s="557"/>
-      <c r="H61" s="558"/>
+      <c r="A61" s="543"/>
+      <c r="B61" s="544"/>
+      <c r="C61" s="545"/>
+      <c r="D61" s="546"/>
+      <c r="E61" s="547"/>
+      <c r="F61" s="548"/>
+      <c r="G61" s="549"/>
+      <c r="H61" s="550"/>
     </row>
     <row r="62">
-      <c r="A62" s="559"/>
-      <c r="B62" s="560"/>
-      <c r="C62" s="561"/>
-      <c r="D62" s="562"/>
-      <c r="E62" s="563"/>
-      <c r="F62" s="564"/>
-      <c r="G62" s="565"/>
-      <c r="H62" s="566"/>
+      <c r="A62" s="551"/>
+      <c r="B62" s="552"/>
+      <c r="C62" s="553"/>
+      <c r="D62" s="554"/>
+      <c r="E62" s="555"/>
+      <c r="F62" s="556"/>
+      <c r="G62" s="557"/>
+      <c r="H62" s="558"/>
     </row>
     <row r="63">
-      <c r="A63" s="567"/>
-      <c r="B63" s="568"/>
-      <c r="C63" s="569"/>
-      <c r="D63" s="570"/>
-      <c r="E63" s="571"/>
-      <c r="F63" s="572"/>
-      <c r="G63" s="573"/>
-      <c r="H63" s="574"/>
+      <c r="A63" s="559"/>
+      <c r="B63" s="560"/>
+      <c r="C63" s="561"/>
+      <c r="D63" s="562"/>
+      <c r="E63" s="563"/>
+      <c r="F63" s="564"/>
+      <c r="G63" s="565"/>
+      <c r="H63" s="566"/>
     </row>
     <row r="64">
-      <c r="A64" s="575"/>
-      <c r="B64" s="576"/>
-      <c r="C64" s="577"/>
-      <c r="D64" s="578"/>
-      <c r="E64" s="579"/>
-      <c r="F64" s="580"/>
-      <c r="G64" s="581"/>
-      <c r="H64" s="582"/>
+      <c r="A64" s="567"/>
+      <c r="B64" s="568"/>
+      <c r="C64" s="569"/>
+      <c r="D64" s="570"/>
+      <c r="E64" s="571"/>
+      <c r="F64" s="572"/>
+      <c r="G64" s="573"/>
+      <c r="H64" s="574"/>
     </row>
     <row r="65">
-      <c r="A65" s="583"/>
-      <c r="B65" s="584"/>
-      <c r="C65" s="585"/>
-      <c r="D65" s="586"/>
-      <c r="E65" s="587"/>
-      <c r="F65" s="588"/>
-      <c r="G65" s="589"/>
-      <c r="H65" s="590"/>
+      <c r="A65" s="575"/>
+      <c r="B65" s="576"/>
+      <c r="C65" s="577"/>
+      <c r="D65" s="578"/>
+      <c r="E65" s="579"/>
+      <c r="F65" s="580"/>
+      <c r="G65" s="581"/>
+      <c r="H65" s="582"/>
     </row>
     <row r="66">
-      <c r="A66" s="591"/>
-      <c r="B66" s="592"/>
-      <c r="C66" s="593"/>
-      <c r="D66" s="594"/>
-      <c r="E66" s="595"/>
-      <c r="F66" s="596"/>
-      <c r="G66" s="597"/>
-      <c r="H66" s="598"/>
+      <c r="A66" s="583"/>
+      <c r="B66" s="584"/>
+      <c r="C66" s="585"/>
+      <c r="D66" s="586"/>
+      <c r="E66" s="587"/>
+      <c r="F66" s="588"/>
+      <c r="G66" s="589"/>
+      <c r="H66" s="590"/>
     </row>
     <row r="67">
-      <c r="A67" s="599"/>
-      <c r="B67" s="600"/>
-      <c r="C67" s="601"/>
-      <c r="D67" s="602"/>
-      <c r="E67" s="603"/>
-      <c r="F67" s="604"/>
-      <c r="G67" s="605"/>
-      <c r="H67" s="606"/>
+      <c r="A67" s="591"/>
+      <c r="B67" s="592"/>
+      <c r="C67" s="593"/>
+      <c r="D67" s="594"/>
+      <c r="E67" s="595"/>
+      <c r="F67" s="596"/>
+      <c r="G67" s="597"/>
+      <c r="H67" s="598"/>
     </row>
     <row r="68">
-      <c r="A68" s="607"/>
-      <c r="B68" s="608"/>
-      <c r="C68" s="609"/>
-      <c r="D68" s="610"/>
-      <c r="E68" s="611"/>
-      <c r="F68" s="612"/>
-      <c r="G68" s="613"/>
-      <c r="H68" s="614"/>
+      <c r="A68" s="599"/>
+      <c r="B68" s="600"/>
+      <c r="C68" s="601"/>
+      <c r="D68" s="602"/>
+      <c r="E68" s="603"/>
+      <c r="F68" s="604"/>
+      <c r="G68" s="605"/>
+      <c r="H68" s="606"/>
     </row>
     <row r="69">
-      <c r="A69" s="615"/>
-      <c r="B69" s="616"/>
-      <c r="C69" s="617"/>
-      <c r="D69" s="618"/>
-      <c r="E69" s="619"/>
-      <c r="F69" s="620"/>
-      <c r="G69" s="621"/>
-      <c r="H69" s="622"/>
+      <c r="A69" s="607"/>
+      <c r="B69" s="608"/>
+      <c r="C69" s="609"/>
+      <c r="D69" s="610"/>
+      <c r="E69" s="611"/>
+      <c r="F69" s="612"/>
+      <c r="G69" s="613"/>
+      <c r="H69" s="614"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="615"/>
+      <c r="B70" s="616"/>
+      <c r="C70" s="617"/>
+      <c r="D70" s="618"/>
+      <c r="E70" s="619"/>
+      <c r="F70" s="620"/>
+      <c r="G70" s="621"/>
+      <c r="H70" s="622"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
Updated to work on 9.1.0000.24350
</commit_message>
<xml_diff>
--- a/TC_CreatePriceList/Main.rvl.xlsx
+++ b/TC_CreatePriceList/Main.rvl.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="167">
   <si>
     <t>Flow</t>
   </si>
@@ -4244,7 +4244,7 @@
     </row>
     <row r="23">
       <c r="A23" s="295" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
       <c r="B23" s="296" t="s">
         <v>3</v>
@@ -4267,7 +4267,9 @@
       <c r="H23" s="302"/>
     </row>
     <row r="24">
-      <c r="A24" s="634"/>
+      <c r="A24" s="634" t="s">
+        <v>127</v>
+      </c>
       <c r="B24" t="s">
         <v>50</v>
       </c>

</xml_diff>